<commit_message>
updates with prf working on current channel!
</commit_message>
<xml_diff>
--- a/protocols/DOSING TABLE_JeanRintoul.xlsx
+++ b/protocols/DOSING TABLE_JeanRintoul.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/pd218_ic_ac_uk/Documents/PhD/Animal stuff/Drugs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ae_mouse\protocols\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F386236B-DE3A-2C4B-BD63-BA342135CE65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9C01F8-E5D4-4B9B-AC44-3D97E0ABFD5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="1155" windowWidth="27990" windowHeight="13920" activeTab="4" xr2:uid="{C223537C-9709-4D08-99CA-5534AD55A010}"/>
+    <workbookView xWindow="1875" yWindow="1530" windowWidth="19065" windowHeight="10740" activeTab="1" xr2:uid="{C223537C-9709-4D08-99CA-5534AD55A010}"/>
   </bookViews>
   <sheets>
     <sheet name="myoverallsheet" sheetId="7" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="104">
   <si>
     <t>Drug</t>
   </si>
@@ -349,6 +349,12 @@
   </si>
   <si>
     <t>dexamethasone SC</t>
+  </si>
+  <si>
+    <t>75mg/ml</t>
+  </si>
+  <si>
+    <t>0.075mg/g</t>
   </si>
 </sst>
 </file>
@@ -487,7 +493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -509,9 +515,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -523,9 +526,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -947,17 +947,17 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="11" t="s">
@@ -981,41 +981,41 @@
       <c r="G11" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="17" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="19">
+      <c r="A12" s="18">
         <v>20</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12" s="19">
         <v>2</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="19">
         <v>1.0000000000000002</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="19">
         <v>0.66315789473684217</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="19">
         <v>6.6666666666666661</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="19">
         <v>2</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="19">
         <f>5*A12/1000/4.5*100/50*100</f>
         <v>4.4444444444444446</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H12" s="19">
         <f>5*A12/1000/4.5*150/50*100</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="19">
         <f>5*A12/1000/4.5*200/50*100</f>
         <v>8.8888888888888893</v>
       </c>
@@ -1039,15 +1039,15 @@
       <c r="F13" s="14">
         <v>2.1999999999999997</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="14">
         <f t="shared" ref="G13:G27" si="0">5*A13/1000/4.5*100/50*100</f>
         <v>4.8888888888888893</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="14">
         <f t="shared" ref="H13:H27" si="1">5*A13/1000/4.5*150/50*100</f>
         <v>7.333333333333333</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="14">
         <f t="shared" ref="I13:I27" si="2">5*A13/1000/4.5*200/50*100</f>
         <v>9.7777777777777786</v>
       </c>
@@ -1071,15 +1071,15 @@
       <c r="F14" s="14">
         <v>2.4</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="14">
         <f t="shared" si="0"/>
         <v>5.333333333333333</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="14">
         <f t="shared" si="1"/>
         <v>7.9999999999999991</v>
       </c>
-      <c r="I14" s="15">
+      <c r="I14" s="14">
         <f t="shared" si="2"/>
         <v>10.666666666666666</v>
       </c>
@@ -1103,15 +1103,15 @@
       <c r="F15" s="14">
         <v>2.6</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="14">
         <f t="shared" si="0"/>
         <v>5.7777777777777786</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="14">
         <f t="shared" si="1"/>
         <v>8.6666666666666679</v>
       </c>
-      <c r="I15" s="15">
+      <c r="I15" s="14">
         <f t="shared" si="2"/>
         <v>11.555555555555557</v>
       </c>
@@ -1135,47 +1135,47 @@
       <c r="F16" s="14">
         <v>2.8000000000000003</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="14">
         <f t="shared" si="0"/>
         <v>6.2222222222222223</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16" s="14">
         <f t="shared" si="1"/>
         <v>9.3333333333333339</v>
       </c>
-      <c r="I16" s="15">
+      <c r="I16" s="14">
         <f t="shared" si="2"/>
         <v>12.444444444444445</v>
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="16">
+      <c r="A17" s="15">
         <v>30</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B17" s="16">
         <v>3</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="16">
         <v>1.5</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="16">
         <v>0.99473684210526314</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="16">
         <v>10</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="16">
         <v>3</v>
       </c>
-      <c r="G17" s="17">
+      <c r="G17" s="16">
         <f>5*A17/1000/4.5*100/50*100</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="H17" s="17">
+      <c r="H17" s="16">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="I17" s="17">
+      <c r="I17" s="16">
         <f t="shared" si="2"/>
         <v>13.333333333333334</v>
       </c>
@@ -1199,15 +1199,15 @@
       <c r="F18" s="14">
         <v>3.2</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G18" s="14">
         <f t="shared" si="0"/>
         <v>7.1111111111111107</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18" s="14">
         <f t="shared" si="1"/>
         <v>10.666666666666666</v>
       </c>
-      <c r="I18" s="15">
+      <c r="I18" s="14">
         <f t="shared" si="2"/>
         <v>14.222222222222221</v>
       </c>
@@ -1231,15 +1231,15 @@
       <c r="F19" s="14">
         <v>3.4000000000000004</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G19" s="14">
         <f t="shared" si="0"/>
         <v>7.5555555555555554</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H19" s="14">
         <f t="shared" si="1"/>
         <v>11.333333333333334</v>
       </c>
-      <c r="I19" s="15">
+      <c r="I19" s="14">
         <f t="shared" si="2"/>
         <v>15.111111111111111</v>
       </c>
@@ -1263,15 +1263,15 @@
       <c r="F20" s="14">
         <v>3.5999999999999996</v>
       </c>
-      <c r="G20" s="15">
+      <c r="G20" s="14">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="H20" s="15">
+      <c r="H20" s="14">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="I20" s="15">
+      <c r="I20" s="14">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
@@ -1295,15 +1295,15 @@
       <c r="F21" s="14">
         <v>3.8</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G21" s="14">
         <f t="shared" si="0"/>
         <v>8.4444444444444446</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21" s="14">
         <f t="shared" si="1"/>
         <v>12.666666666666668</v>
       </c>
-      <c r="I21" s="15">
+      <c r="I21" s="14">
         <f t="shared" si="2"/>
         <v>16.888888888888889</v>
       </c>
@@ -1327,15 +1327,15 @@
       <c r="F22" s="14">
         <v>4</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G22" s="14">
         <f t="shared" si="0"/>
         <v>8.8888888888888893</v>
       </c>
-      <c r="H22" s="15">
+      <c r="H22" s="14">
         <f t="shared" si="1"/>
         <v>13.333333333333334</v>
       </c>
-      <c r="I22" s="15">
+      <c r="I22" s="14">
         <f t="shared" si="2"/>
         <v>17.777777777777779</v>
       </c>
@@ -1359,15 +1359,15 @@
       <c r="F23" s="14">
         <v>4.1999999999999993</v>
       </c>
-      <c r="G23" s="15">
+      <c r="G23" s="14">
         <f t="shared" si="0"/>
         <v>9.3333333333333321</v>
       </c>
-      <c r="H23" s="15">
+      <c r="H23" s="14">
         <f t="shared" si="1"/>
         <v>13.999999999999998</v>
       </c>
-      <c r="I23" s="15">
+      <c r="I23" s="14">
         <f t="shared" si="2"/>
         <v>18.666666666666664</v>
       </c>
@@ -1391,15 +1391,15 @@
       <c r="F24" s="14">
         <v>4.3999999999999995</v>
       </c>
-      <c r="G24" s="15">
+      <c r="G24" s="14">
         <f t="shared" si="0"/>
         <v>9.7777777777777786</v>
       </c>
-      <c r="H24" s="15">
+      <c r="H24" s="14">
         <f t="shared" si="1"/>
         <v>14.666666666666666</v>
       </c>
-      <c r="I24" s="15">
+      <c r="I24" s="14">
         <f t="shared" si="2"/>
         <v>19.555555555555557</v>
       </c>
@@ -1423,15 +1423,15 @@
       <c r="F25" s="14">
         <v>4.5999999999999996</v>
       </c>
-      <c r="G25" s="15">
+      <c r="G25" s="14">
         <f t="shared" si="0"/>
         <v>10.222222222222223</v>
       </c>
-      <c r="H25" s="15">
+      <c r="H25" s="14">
         <f t="shared" si="1"/>
         <v>15.333333333333336</v>
       </c>
-      <c r="I25" s="15">
+      <c r="I25" s="14">
         <f t="shared" si="2"/>
         <v>20.444444444444446</v>
       </c>
@@ -1455,15 +1455,15 @@
       <c r="F26" s="14">
         <v>4.8</v>
       </c>
-      <c r="G26" s="15">
+      <c r="G26" s="14">
         <f t="shared" si="0"/>
         <v>10.666666666666666</v>
       </c>
-      <c r="H26" s="15">
+      <c r="H26" s="14">
         <f t="shared" si="1"/>
         <v>15.999999999999998</v>
       </c>
-      <c r="I26" s="15">
+      <c r="I26" s="14">
         <f t="shared" si="2"/>
         <v>21.333333333333332</v>
       </c>
@@ -1487,15 +1487,15 @@
       <c r="F27" s="14">
         <v>5</v>
       </c>
-      <c r="G27" s="15">
+      <c r="G27" s="14">
         <f t="shared" si="0"/>
         <v>11.111111111111111</v>
       </c>
-      <c r="H27" s="15">
+      <c r="H27" s="14">
         <f t="shared" si="1"/>
         <v>16.666666666666664</v>
       </c>
-      <c r="I27" s="15">
+      <c r="I27" s="14">
         <f t="shared" si="2"/>
         <v>22.222222222222221</v>
       </c>
@@ -1512,8 +1512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{087130FB-B2EC-442E-A99B-3C63BA37434D}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1548,10 +1548,10 @@
         <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1621,16 +1621,16 @@
         <v>0.2</v>
       </c>
       <c r="H7">
-        <f t="shared" ref="H7" si="1">SUM(E7*0.01)</f>
-        <v>0.02</v>
+        <f>SUM(E7*0.0075)</f>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="I7">
         <f>SUM(F7)*0.05</f>
         <v>1.0000000000000002E-2</v>
       </c>
       <c r="K7">
-        <f t="shared" ref="K7" si="2">SUM(H7/0.01)</f>
-        <v>2</v>
+        <f t="shared" ref="K7" si="1">SUM(H7/0.01)</f>
+        <v>1.5</v>
       </c>
       <c r="L7">
         <f>SUM(I7)/0.01</f>
@@ -1649,20 +1649,20 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8:F22" si="3">SUM(C8*0.01)</f>
+        <f t="shared" ref="F8:F22" si="2">SUM(C8*0.01)</f>
         <v>0.22</v>
       </c>
       <c r="H8">
-        <f t="shared" ref="H8:H22" si="4">SUM(E8*0.01)</f>
-        <v>2.2000000000000002E-2</v>
+        <f t="shared" ref="H8:H22" si="3">SUM(E8*0.0075)</f>
+        <v>1.6500000000000001E-2</v>
       </c>
       <c r="I8">
-        <f t="shared" ref="I8:I22" si="5">SUM(F8)*0.05</f>
+        <f t="shared" ref="I8:I22" si="4">SUM(F8)*0.05</f>
         <v>1.1000000000000001E-2</v>
       </c>
       <c r="K8">
-        <f t="shared" ref="K8:K22" si="6">SUM(H8/0.01)</f>
-        <v>2.2000000000000002</v>
+        <f t="shared" ref="K8:K22" si="5">SUM(H8/0.01)</f>
+        <v>1.6500000000000001</v>
       </c>
       <c r="L8">
         <f>SUM(I8)/0.01</f>
@@ -1677,7 +1677,7 @@
         <v>24</v>
       </c>
       <c r="E9">
-        <f t="shared" ref="E9:E22" si="7">SUM(C9)*0.1</f>
+        <f t="shared" ref="E9:E22" si="6">SUM(C9)*0.1</f>
         <v>2.4000000000000004</v>
       </c>
       <c r="F9">
@@ -1685,19 +1685,19 @@
         <v>0.24</v>
       </c>
       <c r="H9">
-        <f t="shared" si="4"/>
-        <v>2.4000000000000004E-2</v>
+        <f t="shared" si="3"/>
+        <v>1.8000000000000002E-2</v>
       </c>
       <c r="I9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.2E-2</v>
       </c>
       <c r="K9">
-        <f t="shared" si="6"/>
-        <v>2.4000000000000004</v>
+        <f t="shared" si="5"/>
+        <v>1.8000000000000003</v>
       </c>
       <c r="L9">
-        <f t="shared" ref="L9:L22" si="8">SUM(I9)/0.01</f>
+        <f t="shared" ref="L9:L22" si="7">SUM(I9)/0.01</f>
         <v>1.2</v>
       </c>
       <c r="M9">
@@ -1709,27 +1709,27 @@
         <v>26</v>
       </c>
       <c r="E10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>2.6</v>
       </c>
       <c r="F10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.26</v>
       </c>
       <c r="H10">
-        <f t="shared" si="4"/>
-        <v>2.6000000000000002E-2</v>
+        <f t="shared" si="3"/>
+        <v>1.95E-2</v>
       </c>
       <c r="I10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.3000000000000001E-2</v>
       </c>
       <c r="K10">
-        <f t="shared" si="6"/>
-        <v>2.6</v>
+        <f t="shared" si="5"/>
+        <v>1.95</v>
       </c>
       <c r="L10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1.3</v>
       </c>
       <c r="M10">
@@ -1741,27 +1741,27 @@
         <v>28</v>
       </c>
       <c r="E11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>2.8000000000000003</v>
       </c>
       <c r="F11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.28000000000000003</v>
       </c>
       <c r="H11">
-        <f t="shared" si="4"/>
-        <v>2.8000000000000004E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="I11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.4000000000000002E-2</v>
       </c>
       <c r="K11">
-        <f t="shared" si="6"/>
-        <v>2.8000000000000003</v>
+        <f t="shared" si="5"/>
+        <v>2.1</v>
       </c>
       <c r="L11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1.4000000000000001</v>
       </c>
       <c r="M11">
@@ -1773,27 +1773,27 @@
         <v>30</v>
       </c>
       <c r="E12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="F12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.3</v>
       </c>
       <c r="H12">
-        <f t="shared" si="4"/>
-        <v>0.03</v>
+        <f t="shared" si="3"/>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="I12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="K12">
-        <f t="shared" si="6"/>
-        <v>3</v>
+        <f t="shared" si="5"/>
+        <v>2.25</v>
       </c>
       <c r="L12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1.5</v>
       </c>
       <c r="M12">
@@ -1805,27 +1805,27 @@
         <v>32</v>
       </c>
       <c r="E13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>3.2</v>
       </c>
       <c r="F13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.32</v>
       </c>
       <c r="H13">
-        <f t="shared" si="4"/>
-        <v>3.2000000000000001E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.4E-2</v>
       </c>
       <c r="I13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.6E-2</v>
       </c>
       <c r="K13">
-        <f t="shared" si="6"/>
-        <v>3.2</v>
+        <f t="shared" si="5"/>
+        <v>2.4</v>
       </c>
       <c r="L13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1.6</v>
       </c>
       <c r="M13">
@@ -1837,27 +1837,27 @@
         <v>34</v>
       </c>
       <c r="E14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>3.4000000000000004</v>
       </c>
       <c r="F14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.34</v>
       </c>
       <c r="H14">
-        <f t="shared" si="4"/>
-        <v>3.4000000000000002E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.5500000000000002E-2</v>
       </c>
       <c r="I14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="K14">
-        <f t="shared" si="6"/>
-        <v>3.4000000000000004</v>
+        <f t="shared" si="5"/>
+        <v>2.5500000000000003</v>
       </c>
       <c r="L14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1.7000000000000002</v>
       </c>
       <c r="M14">
@@ -1869,27 +1869,27 @@
         <v>36</v>
       </c>
       <c r="E15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>3.6</v>
       </c>
       <c r="F15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.36</v>
       </c>
       <c r="H15">
-        <f t="shared" si="4"/>
-        <v>3.6000000000000004E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.7E-2</v>
       </c>
       <c r="I15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="K15">
-        <f t="shared" si="6"/>
-        <v>3.6000000000000005</v>
+        <f t="shared" si="5"/>
+        <v>2.6999999999999997</v>
       </c>
       <c r="L15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1.7999999999999998</v>
       </c>
       <c r="M15">
@@ -1901,27 +1901,27 @@
         <v>38</v>
       </c>
       <c r="E16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>3.8000000000000003</v>
       </c>
       <c r="F16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.38</v>
       </c>
       <c r="H16">
-        <f t="shared" si="4"/>
-        <v>3.8000000000000006E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.8500000000000001E-2</v>
       </c>
       <c r="I16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.9000000000000003E-2</v>
       </c>
       <c r="K16">
-        <f t="shared" si="6"/>
-        <v>3.8000000000000007</v>
+        <f t="shared" si="5"/>
+        <v>2.85</v>
       </c>
       <c r="L16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1.9000000000000004</v>
       </c>
       <c r="M16">
@@ -1933,27 +1933,27 @@
         <v>40</v>
       </c>
       <c r="E17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="F17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
       <c r="H17">
-        <f t="shared" si="4"/>
-        <v>0.04</v>
+        <f t="shared" si="3"/>
+        <v>0.03</v>
       </c>
       <c r="I17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.0000000000000004E-2</v>
       </c>
       <c r="K17">
-        <f t="shared" si="6"/>
-        <v>4</v>
+        <f t="shared" si="5"/>
+        <v>3</v>
       </c>
       <c r="L17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2.0000000000000004</v>
       </c>
       <c r="M17">
@@ -1965,27 +1965,27 @@
         <v>42</v>
       </c>
       <c r="E18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>4.2</v>
       </c>
       <c r="F18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.42</v>
       </c>
       <c r="H18">
-        <f t="shared" si="4"/>
-        <v>4.2000000000000003E-2</v>
+        <f t="shared" si="3"/>
+        <v>3.15E-2</v>
       </c>
       <c r="I18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="K18">
-        <f t="shared" si="6"/>
-        <v>4.2</v>
+        <f t="shared" si="5"/>
+        <v>3.15</v>
       </c>
       <c r="L18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2.1</v>
       </c>
       <c r="M18">
@@ -1997,27 +1997,27 @@
         <v>44</v>
       </c>
       <c r="E19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="F19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.44</v>
       </c>
       <c r="H19">
-        <f t="shared" si="4"/>
-        <v>4.4000000000000004E-2</v>
+        <f t="shared" si="3"/>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="I19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.2000000000000002E-2</v>
       </c>
       <c r="K19">
-        <f t="shared" si="6"/>
-        <v>4.4000000000000004</v>
+        <f t="shared" si="5"/>
+        <v>3.3000000000000003</v>
       </c>
       <c r="L19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="M19">
@@ -2029,27 +2029,27 @@
         <v>46</v>
       </c>
       <c r="E20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>4.6000000000000005</v>
       </c>
       <c r="F20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.46</v>
       </c>
       <c r="H20">
-        <f t="shared" si="4"/>
-        <v>4.6000000000000006E-2</v>
+        <f t="shared" si="3"/>
+        <v>3.4500000000000003E-2</v>
       </c>
       <c r="I20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.3000000000000003E-2</v>
       </c>
       <c r="K20">
-        <f t="shared" si="6"/>
-        <v>4.6000000000000005</v>
+        <f t="shared" si="5"/>
+        <v>3.45</v>
       </c>
       <c r="L20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2.3000000000000003</v>
       </c>
       <c r="M20">
@@ -2061,27 +2061,27 @@
         <v>48</v>
       </c>
       <c r="E21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>4.8000000000000007</v>
       </c>
       <c r="F21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.48</v>
       </c>
       <c r="H21">
-        <f t="shared" si="4"/>
-        <v>4.8000000000000008E-2</v>
+        <f t="shared" si="3"/>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="I21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.4E-2</v>
       </c>
       <c r="K21">
-        <f t="shared" si="6"/>
-        <v>4.8000000000000007</v>
+        <f t="shared" si="5"/>
+        <v>3.6000000000000005</v>
       </c>
       <c r="L21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2.4</v>
       </c>
       <c r="M21">
@@ -2093,27 +2093,27 @@
         <v>50</v>
       </c>
       <c r="E22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="F22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="H22">
-        <f t="shared" si="4"/>
-        <v>0.05</v>
+        <f t="shared" si="3"/>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="I22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="K22">
-        <f t="shared" si="6"/>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>3.75</v>
       </c>
       <c r="L22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
       <c r="M22">
@@ -3660,8 +3660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9860FA5F-D6D4-48C3-8E0A-CCE7CD0085C5}">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>